<commit_message>
edit code and put figures
</commit_message>
<xml_diff>
--- a/data/bali-station.xlsx
+++ b/data/bali-station.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fsari2/Documents/UIUC/ATMS523/Module8/machine-learning-application/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A3BC363-5EB2-AF4A-967A-7F65DDE96322}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2E11135-08EC-3245-AA31-7A64FBD84AAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="1280" windowWidth="27240" windowHeight="15460" xr2:uid="{97D1CCB2-43C5-134E-958E-C98235EC263D}"/>
   </bookViews>
@@ -428,7 +428,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -467,31 +467,67 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>-8.3444000000000003</v>
+      </c>
+      <c r="B4">
+        <v>114.6272</v>
+      </c>
       <c r="C4" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>-8.7227490000000003</v>
+      </c>
+      <c r="B5">
+        <v>115.16970000000001</v>
+      </c>
       <c r="C5" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>-8.7465360000000008</v>
+      </c>
+      <c r="B6">
+        <v>115.211375</v>
+      </c>
       <c r="C6" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>-8.4608333299999998</v>
+      </c>
+      <c r="B7">
+        <v>115.13966670000001</v>
+      </c>
       <c r="C7" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>-8.4159799999999994</v>
+      </c>
+      <c r="B8">
+        <v>115.42010000000001</v>
+      </c>
       <c r="C8" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>-8.5421600000000009</v>
+      </c>
+      <c r="B9">
+        <v>115.441</v>
+      </c>
       <c r="C9" s="2" t="s">
         <v>10</v>
       </c>

</xml_diff>